<commit_message>
added term accession numbers to ambiguous tags and harmonized similar tags
</commit_message>
<xml_diff>
--- a/templates/community/MAdLand/MAdLand_sample_sheets.xlsx
+++ b/templates/community/MAdLand/MAdLand_sample_sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\MAdLand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8F608C-CDA9-467F-A5E8-00B6AD2AE70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8372EE-BFFA-45E1-B20F-4CEDA1EF1E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{D3EB6A5A-F5C7-441F-91D4-3808AE23C83B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D3EB6A5A-F5C7-441F-91D4-3808AE23C83B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample information" sheetId="1" r:id="rId1"/>
@@ -50,75 +50,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AFAC9482-5B1B-4047-96FF-8E343FAFAA16}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=bac2606c-ac54-4abf-8a76-257bdc777e4d</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{378D63A7-4B55-4EC7-AC00-DCA67A86B4A3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{46B5F1FA-A49E-4609-9A85-F43E892222E4}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{8DC5B03A-A150-4C9A-8134-CAC922482A26}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{0E4B40E6-3AA6-4BC6-BAC6-64536A89B2DC}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{2DB4CE41-E6E9-4A01-8E91-48AD04EC602A}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{A2955A8A-2890-4BF1-AE51-8090DC2E0721}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{3E4D436F-64AB-4B66-BF16-859DD6CAEB18}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{5C4C7881-A516-4297-91A6-C38AA950E52D}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Source Name</t>
   </si>
@@ -325,13 +325,19 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C14258</t>
+  </si>
+  <si>
+    <t>NCIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,12 +360,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -511,8 +511,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,9 +570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -610,7 +610,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -716,7 +716,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -858,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -938,37 +938,37 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="42.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.42578125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="39.5703125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="42.44140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.44140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="43.6640625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R8" t="s">
         <v>20</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R9" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R10" t="s">
         <v>20</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R11" t="s">
         <v>20</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R12" t="s">
         <v>20</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R13" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="R14" t="s">
         <v>20</v>
       </c>
@@ -1117,17 +1117,17 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1175,31 +1175,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1221,29 +1221,33 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -1251,7 +1255,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1259,13 +1263,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1273,49 +1277,49 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>65</v>
       </c>

</xml_diff>